<commit_message>
The 6a report was done
</commit_message>
<xml_diff>
--- a/backend/reports/a6.xlsx
+++ b/backend/reports/a6.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Хужайли туманидаги мелиоратив кудуклардаги ер ости сувларини жойлашиши хакида </t>
   </si>
@@ -56,12 +56,6 @@
     <t xml:space="preserve">  уртача чукурлиги   см</t>
   </si>
   <si>
-    <t>2020 й ноябрь уртача чукурлиги см</t>
-  </si>
-  <si>
-    <t>хизмат киладиган майдони га</t>
-  </si>
-  <si>
     <t>Дно скважин в см</t>
   </si>
   <si>
@@ -75,18 +69,6 @@
   </si>
   <si>
     <t>III</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0 - 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 - 1,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1,5 - 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> более 2м</t>
   </si>
 </sst>
 </file>
@@ -189,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -197,40 +179,47 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,60 +501,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="7"/>
-    <col min="2" max="3" width="8.88671875" style="8"/>
-    <col min="4" max="16" width="8.88671875" style="7"/>
+    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="2" max="3" width="8.88671875" style="6"/>
+    <col min="4" max="12" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -576,147 +557,109 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
+      <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="9" t="s">
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="15"/>
+      <c r="K4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="L4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="9" t="s">
+    </row>
+    <row r="5" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="G5" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="H5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
     </row>
-    <row r="5" spans="1:16" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="4" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4</v>
+      </c>
+      <c r="F6" s="3">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4">
+        <v>6</v>
+      </c>
+      <c r="H6" s="4">
+        <v>7</v>
+      </c>
+      <c r="I6" s="4">
+        <v>8</v>
+      </c>
+      <c r="J6" s="4">
+        <v>9</v>
+      </c>
+      <c r="K6" s="4">
         <v>14</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5">
-        <v>3</v>
-      </c>
-      <c r="E6" s="5">
-        <v>4</v>
-      </c>
-      <c r="F6" s="4">
-        <v>5</v>
-      </c>
-      <c r="G6" s="5">
-        <v>6</v>
-      </c>
-      <c r="H6" s="5">
-        <v>7</v>
-      </c>
-      <c r="I6" s="5">
-        <v>8</v>
-      </c>
-      <c r="J6" s="5">
-        <v>9</v>
-      </c>
-      <c r="K6" s="5">
-        <v>10</v>
-      </c>
-      <c r="L6" s="5">
-        <v>11</v>
-      </c>
-      <c r="M6" s="5">
-        <v>12</v>
-      </c>
-      <c r="N6" s="5">
-        <v>13</v>
-      </c>
-      <c r="O6" s="5">
-        <v>14</v>
-      </c>
-      <c r="P6" s="6">
+      <c r="L6" s="9">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="N3:P3"/>
+  <mergeCells count="10">
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="K3:L3"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="I4:I5"/>
   </mergeCells>

</xml_diff>